<commit_message>
Add constraint examples to ingrowth form.
</commit_message>
<xml_diff>
--- a/odk_app/config/tables/ingrowth/forms/ingrowth/ingrowth.xlsx
+++ b/odk_app/config/tables/ingrowth/forms/ingrowth/ingrowth.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Home\dev\classes\capstone\app-designer-2.1.6\app\config\tables\ingrowth\forms\ingrowth\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joey\Desktop\dev\classes\capstone\app-designer-2.1.6\app\config\tables\ingrowth\forms\ingrowth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF709E5-F8C8-4370-BFE8-72996F5495C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1A5DDD-29AA-458B-9D2F-CF58C9152D93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="38640" windowHeight="21390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="281">
   <si>
     <t>clause</t>
   </si>
@@ -847,6 +847,30 @@
   </si>
   <si>
     <t>TSME - Tsuga mertensiana (mountain hemlock)</t>
+  </si>
+  <si>
+    <t>constraint</t>
+  </si>
+  <si>
+    <t>display.constraint_message.text</t>
+  </si>
+  <si>
+    <t>if</t>
+  </si>
+  <si>
+    <t>end if</t>
+  </si>
+  <si>
+    <t>DBH != 123.</t>
+  </si>
+  <si>
+    <t>data('dbh') != 123</t>
+  </si>
+  <si>
+    <t>Dbh isnt right.</t>
+  </si>
+  <si>
+    <t>(function() { if (data('dbh') == "123") { return true;} alert('DBH incorrect'); return false;}) ()</t>
   </si>
 </sst>
 </file>
@@ -1332,23 +1356,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="81.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1367,13 +1393,19 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>273</v>
+      </c>
+      <c r="H1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>38</v>
       </c>
@@ -1384,7 +1416,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>38</v>
       </c>
@@ -1395,7 +1427,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>207</v>
       </c>
@@ -1409,7 +1441,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>15</v>
       </c>
@@ -1419,138 +1451,135 @@
       <c r="F6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>208</v>
-      </c>
-      <c r="D7" t="s">
-        <v>84</v>
-      </c>
-      <c r="E7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>280</v>
+      </c>
+      <c r="H6" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>275</v>
+      </c>
+      <c r="B7" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>207</v>
-      </c>
-      <c r="D8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>208</v>
       </c>
       <c r="D10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>207</v>
+      </c>
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>208</v>
+      </c>
+      <c r="D13" t="s">
         <v>98</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E13" t="s">
         <v>53</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
         <v>208</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D14" t="s">
         <v>55</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E14" t="s">
         <v>55</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F14" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
         <v>208</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D15" t="s">
         <v>57</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E15" t="s">
         <v>57</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F15" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
         <v>15</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E16" t="s">
         <v>59</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F16" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" t="s">
-        <v>61</v>
-      </c>
-      <c r="F14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" t="s">
-        <v>62</v>
-      </c>
-      <c r="F15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="E17" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F17" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1558,91 +1587,122 @@
         <v>15</v>
       </c>
       <c r="E18" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F18" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" t="s">
-        <v>70</v>
+        <v>17</v>
       </c>
       <c r="F19" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>17</v>
+        <v>38</v>
+      </c>
+      <c r="E20" t="s">
+        <v>66</v>
       </c>
       <c r="F20" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>207</v>
-      </c>
-      <c r="D21" t="s">
-        <v>108</v>
+        <v>15</v>
       </c>
       <c r="E21" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F21" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>207</v>
-      </c>
-      <c r="D22" t="s">
-        <v>108</v>
+        <v>15</v>
       </c>
       <c r="E22" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F22" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>207</v>
-      </c>
-      <c r="D23" t="s">
-        <v>108</v>
-      </c>
-      <c r="E23" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="F23" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
+        <v>207</v>
+      </c>
+      <c r="D24" t="s">
+        <v>108</v>
+      </c>
+      <c r="E24" t="s">
+        <v>73</v>
+      </c>
+      <c r="F24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>207</v>
+      </c>
+      <c r="D25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E25" t="s">
+        <v>75</v>
+      </c>
+      <c r="F25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>207</v>
+      </c>
+      <c r="D26" t="s">
+        <v>108</v>
+      </c>
+      <c r="E26" t="s">
+        <v>77</v>
+      </c>
+      <c r="F26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
         <v>79</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E27" t="s">
         <v>80</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F27" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>